<commit_message>
Reset vouchers.xlsx (clear all data)
</commit_message>
<xml_diff>
--- a/vouchers.xlsx
+++ b/vouchers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,121 +436,30 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>phone</t>
+          <t>voucher_code</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>code</t>
+          <t>phone</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>points_cost</t>
+          <t>value</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>amount</t>
+          <t>issued_ts</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>issued_ts</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>redeemed</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>redeemed_ts</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>79174445</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>V4445-100-5-20250818174229</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-08-18T17:42:29</t>
-        </is>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025-08-18T17:44:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>79174445</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>V4445-500-40-20250818174328</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>500</v>
-      </c>
-      <c r="D3" t="n">
-        <v>40</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-08-18T17:43:28</t>
-        </is>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>71076783</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>V6783-100-5-20250818175048</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>100</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2025-08-18T17:50:48</t>
-        </is>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>